<commit_message>
date extractor done, settings changed
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,33 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lroland\Desktop\Lucile\Année 2021 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luaroncrew/PycharmProjects/university_agenda_to_apple_calendar/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BDEB6F-6ADD-6541-9AFE-D5F70C3D1A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="495" windowWidth="27720" windowHeight="17505"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semaine 37 - 2021" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="56">
   <si>
     <t>Année</t>
   </si>
   <si>
     <t>IUT Lumière</t>
-  </si>
-  <si>
-    <t>09/09/2021</t>
   </si>
   <si>
     <t>Semaine</t>
@@ -287,8 +296,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -928,6 +937,81 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -946,103 +1030,28 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1353,343 +1362,337 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="29" width="5.85546875" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="5.7109375" style="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6" max="29" width="5.83203125" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="5.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75">
+    <row r="1" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3">
         <v>2021</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="59" t="s">
+      <c r="G1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59" t="s">
+      <c r="H1" s="52"/>
+      <c r="I1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59" t="s">
+      <c r="K1" s="52"/>
+      <c r="L1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="59" t="s">
+      <c r="N1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="59" t="s">
+      <c r="O1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="59" t="s">
+      <c r="P1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="59" t="s">
+      <c r="Q1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="59" t="s">
+      <c r="R1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="59" t="s">
+      <c r="S1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="T1" s="59" t="s">
+      <c r="T1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="59" t="s">
+      <c r="U1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="58" t="s">
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+    </row>
+    <row r="2" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="AB1" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC1" s="58" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" ht="15.75">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="B2" s="3">
         <v>37</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="U2" s="53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="P2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="S2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="T2" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2" s="60" t="s">
-        <v>4</v>
-      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
     </row>
-    <row r="3" spans="1:29" ht="15.75">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="B6" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="R3" s="60"/>
-      <c r="S3" s="60"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="60"/>
+      <c r="C6" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="S6" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="T6" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="U6" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="V6" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="X6" s="62"/>
+      <c r="Y6" s="62"/>
+      <c r="Z6" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA6" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB6" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC6" s="62" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:29">
-      <c r="B6" s="66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="66" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="66" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="P6" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="R6" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="S6" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="T6" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="U6" s="66" t="s">
-        <v>10</v>
-      </c>
-      <c r="V6" s="66" t="s">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="B7" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="W6" s="66" t="s">
+      <c r="C7" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="X6" s="66"/>
-      <c r="Y6" s="66"/>
-      <c r="Z6" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA6" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB6" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC6" s="66" t="s">
-        <v>11</v>
+      <c r="D7" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="S7" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="U7" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="V7" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="W7" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="63"/>
+      <c r="Z7" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA7" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB7" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC7" s="63" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
-      <c r="B7" s="67" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="67" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="N7" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="O7" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="P7" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q7" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="R7" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="S7" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="T7" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="U7" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="V7" s="67" t="s">
+    <row r="8" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="W7" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="X7" s="67"/>
-      <c r="Y7" s="67"/>
-      <c r="Z7" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA7" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB7" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC7" s="67" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" ht="21.95" customHeight="1">
-      <c r="A8" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="32"/>
+      <c r="B8" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="57"/>
       <c r="F8" s="13"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -1698,57 +1701,57 @@
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="15"/>
-      <c r="N8" s="46" t="s">
+      <c r="N8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="T8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="U8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="V8" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="P8" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q8" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="R8" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="S8" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="T8" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="U8" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="V8" s="37" t="s">
+      <c r="W8" s="42"/>
+      <c r="X8" s="42"/>
+      <c r="Y8" s="67"/>
+      <c r="Z8" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="W8" s="38"/>
-      <c r="X8" s="38"/>
-      <c r="Y8" s="39"/>
-      <c r="Z8" s="46" t="s">
+      <c r="AA8" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="AA8" s="46" t="s">
+      <c r="AC8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="AB8" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC8" s="46" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="9" spans="1:29" ht="21.95" customHeight="1">
+    <row r="9" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="34"/>
+        <v>16</v>
+      </c>
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="59"/>
       <c r="F9" s="16"/>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
@@ -1757,394 +1760,394 @@
       <c r="K9" s="26"/>
       <c r="L9" s="26"/>
       <c r="M9" s="27"/>
-      <c r="N9" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="O9" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q9" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="R9" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="S9" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="T9" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="U9" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="V9" s="40"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="41"/>
-      <c r="Y9" s="42"/>
-      <c r="Z9" s="46" t="s">
+      <c r="N9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="R9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="T9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="U9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="V9" s="35"/>
+      <c r="W9" s="36"/>
+      <c r="X9" s="36"/>
+      <c r="Y9" s="37"/>
+      <c r="Z9" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA9" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB9" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="AA9" s="46" t="s">
+      <c r="AC9" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="AB9" s="46" t="s">
+    </row>
+    <row r="10" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="AC9" s="46" t="s">
+      <c r="B10" s="58"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="31"/>
+      <c r="I10" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q10" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="R10" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="S10" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="T10" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="U10" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="V10" s="35"/>
+      <c r="W10" s="36"/>
+      <c r="X10" s="36"/>
+      <c r="Y10" s="37"/>
+      <c r="Z10" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA10" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB10" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC10" s="31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="65" t="s">
         <v>21</v>
       </c>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="31"/>
+      <c r="I11" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="44"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="R11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="S11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="T11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="U11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="V11" s="38"/>
+      <c r="W11" s="39"/>
+      <c r="X11" s="39"/>
+      <c r="Y11" s="40"/>
+      <c r="Z11" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA11" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB11" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC11" s="31" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="10" spans="1:29" ht="21.95" customHeight="1">
-      <c r="A10" s="65" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="46"/>
-      <c r="I10" s="64" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="50" t="s">
+    <row r="12" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="O10" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q10" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="R10" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="S10" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="T10" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="U10" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="V10" s="40"/>
-      <c r="W10" s="41"/>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="42"/>
-      <c r="Z10" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA10" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB10" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC10" s="46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" ht="21.95" customHeight="1">
-      <c r="A11" s="65" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="46"/>
-      <c r="I11" s="64" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="52"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="O11" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="P11" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q11" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="R11" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="S11" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="T11" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="U11" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="V11" s="43"/>
-      <c r="W11" s="44"/>
-      <c r="X11" s="44"/>
-      <c r="Y11" s="45"/>
-      <c r="Z11" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA11" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB11" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC11" s="46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" ht="21.95" customHeight="1">
-      <c r="A12" s="65" t="s">
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="46" t="s">
-        <v>26</v>
+      <c r="G12" s="31" t="s">
+        <v>25</v>
       </c>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="61" t="s">
+      <c r="J12" s="44"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="S12" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="T12" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="O12" s="48"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="S12" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="T12" s="46" t="s">
+      <c r="U12" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="V12" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="U12" s="46" t="s">
+      <c r="W12" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="V12" s="46" t="s">
+      <c r="X12" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="W12" s="46" t="s">
+      <c r="Y12" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="X12" s="46" t="s">
+      <c r="Z12" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="Y12" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z12" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA12" s="48"/>
-      <c r="AB12" s="48"/>
-      <c r="AC12" s="49"/>
+      <c r="AA12" s="33"/>
+      <c r="AB12" s="33"/>
+      <c r="AC12" s="34"/>
     </row>
-    <row r="13" spans="1:29" ht="21.95" customHeight="1">
+    <row r="13" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="58"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="46" t="s">
-        <v>26</v>
+      <c r="G13" s="31" t="s">
+        <v>25</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="S13" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="T13" s="46" t="s">
+      <c r="J13" s="44"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="S13" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="T13" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="U13" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="V13" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="U13" s="46" t="s">
+      <c r="W13" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="V13" s="46" t="s">
+      <c r="X13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="W13" s="46" t="s">
+      <c r="Y13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="X13" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y13" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z13" s="40"/>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="41"/>
-      <c r="AC13" s="42"/>
+      <c r="Z13" s="35"/>
+      <c r="AA13" s="36"/>
+      <c r="AB13" s="36"/>
+      <c r="AC13" s="37"/>
     </row>
-    <row r="14" spans="1:29" ht="21.95" customHeight="1">
+    <row r="14" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="46" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="B14" s="58"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>25</v>
       </c>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="S14" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="T14" s="46" t="s">
+      <c r="J14" s="44"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="S14" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="T14" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="U14" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="V14" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="U14" s="46" t="s">
+      <c r="W14" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="V14" s="46" t="s">
+      <c r="X14" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="W14" s="46" t="s">
+      <c r="Y14" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="X14" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y14" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z14" s="40"/>
-      <c r="AA14" s="41"/>
-      <c r="AB14" s="41"/>
-      <c r="AC14" s="42"/>
+      <c r="Z14" s="35"/>
+      <c r="AA14" s="36"/>
+      <c r="AB14" s="36"/>
+      <c r="AC14" s="37"/>
     </row>
-    <row r="15" spans="1:29" ht="21.95" customHeight="1">
+    <row r="15" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="46" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="B15" s="60"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>25</v>
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="55"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="62"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="S15" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="T15" s="46" t="s">
+      <c r="J15" s="46"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="S15" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="T15" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="U15" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="V15" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="U15" s="46" t="s">
+      <c r="W15" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="V15" s="46" t="s">
+      <c r="X15" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="W15" s="46" t="s">
+      <c r="Y15" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="X15" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y15" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z15" s="43"/>
-      <c r="AA15" s="44"/>
-      <c r="AB15" s="44"/>
-      <c r="AC15" s="45"/>
+      <c r="Z15" s="38"/>
+      <c r="AA15" s="39"/>
+      <c r="AB15" s="39"/>
+      <c r="AC15" s="40"/>
     </row>
-    <row r="16" spans="1:29" ht="21.95" customHeight="1">
+    <row r="16" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="65" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
@@ -2175,9 +2178,9 @@
       <c r="AB16" s="20"/>
       <c r="AC16" s="21"/>
     </row>
-    <row r="17" spans="1:29" ht="21.95" customHeight="1">
+    <row r="17" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="65" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
@@ -2208,9 +2211,9 @@
       <c r="AB17" s="20"/>
       <c r="AC17" s="21"/>
     </row>
-    <row r="18" spans="1:29" ht="21.95" customHeight="1">
+    <row r="18" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="65" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
@@ -2241,372 +2244,372 @@
       <c r="AB18" s="20"/>
       <c r="AC18" s="21"/>
     </row>
-    <row r="19" spans="1:29" ht="21.95" customHeight="1">
+    <row r="19" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="57"/>
+      <c r="D19" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="57"/>
+      <c r="F19" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="50" t="s">
+      <c r="K19" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="K19" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="N19" s="46" t="s">
+      <c r="O19" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="P19" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="O19" s="46" t="s">
+      <c r="Q19" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="P19" s="46" t="s">
+      <c r="R19" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="Q19" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="R19" s="50" t="s">
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="43"/>
+      <c r="V19" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="51"/>
-      <c r="V19" s="57" t="s">
+      <c r="W19" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="X19" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="W19" s="46" t="s">
+      <c r="Y19" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="X19" s="46" t="s">
+      <c r="Z19" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="Y19" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z19" s="47" t="s">
+      <c r="AA19" s="33"/>
+      <c r="AB19" s="33"/>
+      <c r="AC19" s="34"/>
+    </row>
+    <row r="20" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="AA19" s="48"/>
-      <c r="AB19" s="48"/>
-      <c r="AC19" s="49"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="N20" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="O20" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="P20" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q20" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="R20" s="44"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="36"/>
+      <c r="U20" s="45"/>
+      <c r="V20" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="W20" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="X20" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y20" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z20" s="35"/>
+      <c r="AA20" s="36"/>
+      <c r="AB20" s="36"/>
+      <c r="AC20" s="37"/>
     </row>
-    <row r="20" spans="1:29" ht="21.95" customHeight="1">
-      <c r="A20" s="65" t="s">
+    <row r="21" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="K20" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="L20" s="46"/>
-      <c r="M20" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="N20" s="46" t="s">
+      <c r="K21" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="N21" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="O21" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="P21" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="O20" s="46" t="s">
+      <c r="Q21" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="P20" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q20" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="R20" s="52"/>
-      <c r="S20" s="41"/>
-      <c r="T20" s="41"/>
-      <c r="U20" s="53"/>
-      <c r="V20" s="57" t="s">
+      <c r="R21" s="44"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="45"/>
+      <c r="V21" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="W21" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="X21" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="W20" s="46" t="s">
+      <c r="Y21" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="X20" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y20" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z20" s="40"/>
-      <c r="AA20" s="41"/>
-      <c r="AB20" s="41"/>
-      <c r="AC20" s="42"/>
+      <c r="Z21" s="35"/>
+      <c r="AA21" s="36"/>
+      <c r="AB21" s="36"/>
+      <c r="AC21" s="37"/>
     </row>
-    <row r="21" spans="1:29" ht="21.95" customHeight="1">
-      <c r="A21" s="65" t="s">
+    <row r="22" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="57" t="s">
+      <c r="K22" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="N22" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="O22" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="P22" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q22" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="R22" s="46"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="47"/>
+      <c r="U22" s="48"/>
+      <c r="V22" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="W22" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="X22" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y22" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z22" s="38"/>
+      <c r="AA22" s="39"/>
+      <c r="AB22" s="39"/>
+      <c r="AC22" s="40"/>
+    </row>
+    <row r="23" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="K21" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="L21" s="46"/>
-      <c r="M21" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="N21" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="O21" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="P21" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q21" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="R21" s="52"/>
-      <c r="S21" s="41"/>
-      <c r="T21" s="41"/>
-      <c r="U21" s="53"/>
-      <c r="V21" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="W21" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="X21" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y21" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z21" s="40"/>
-      <c r="AA21" s="41"/>
-      <c r="AB21" s="41"/>
-      <c r="AC21" s="42"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="K23" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="N23" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="O23" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="P23" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q23" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="R23" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="S23" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="T23" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="U23" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="V23" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="W23" s="33"/>
+      <c r="X23" s="33"/>
+      <c r="Y23" s="34"/>
+      <c r="Z23" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA23" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB23" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC23" s="31" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="22" spans="1:29" ht="21.95" customHeight="1">
-      <c r="A22" s="65" t="s">
+    <row r="24" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="N24" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="O24" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="P24" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q24" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="R24" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="S24" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="T24" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="K22" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="L22" s="46"/>
-      <c r="M22" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="N22" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="O22" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="P22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q22" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="R22" s="54"/>
-      <c r="S22" s="55"/>
-      <c r="T22" s="55"/>
-      <c r="U22" s="56"/>
-      <c r="V22" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="W22" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="X22" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y22" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z22" s="43"/>
-      <c r="AA22" s="44"/>
-      <c r="AB22" s="44"/>
-      <c r="AC22" s="45"/>
+      <c r="U24" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="V24" s="35"/>
+      <c r="W24" s="36"/>
+      <c r="X24" s="36"/>
+      <c r="Y24" s="37"/>
+      <c r="Z24" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA24" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB24" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC24" s="31" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="23" spans="1:29" ht="21.95" customHeight="1">
-      <c r="A23" s="65" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="K23" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="N23" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="O23" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="P23" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q23" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="R23" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="S23" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="T23" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="U23" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="V23" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="W23" s="48"/>
-      <c r="X23" s="48"/>
-      <c r="Y23" s="49"/>
-      <c r="Z23" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA23" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB23" s="46" t="s">
+    <row r="25" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="AC23" s="46" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" ht="21.95" customHeight="1">
-      <c r="A24" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="K24" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="L24" s="46"/>
-      <c r="M24" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="N24" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="O24" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="P24" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q24" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="R24" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="S24" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="T24" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="U24" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="V24" s="40"/>
-      <c r="W24" s="41"/>
-      <c r="X24" s="41"/>
-      <c r="Y24" s="42"/>
-      <c r="Z24" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA24" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB24" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC24" s="46" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" ht="21.95" customHeight="1">
-      <c r="A25" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="34"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
       <c r="F25" s="24"/>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
@@ -2615,55 +2618,55 @@
       <c r="K25" s="17"/>
       <c r="L25" s="17"/>
       <c r="M25" s="18"/>
-      <c r="N25" s="46" t="s">
+      <c r="N25" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="O25" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="P25" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="O25" s="46" t="s">
+      <c r="Q25" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P25" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q25" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="R25" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="S25" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="T25" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="U25" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="V25" s="40"/>
-      <c r="W25" s="41"/>
-      <c r="X25" s="41"/>
-      <c r="Y25" s="42"/>
-      <c r="Z25" s="46" t="s">
+      <c r="R25" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="S25" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="T25" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="U25" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="V25" s="35"/>
+      <c r="W25" s="36"/>
+      <c r="X25" s="36"/>
+      <c r="Y25" s="37"/>
+      <c r="Z25" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA25" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB25" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="AA25" s="46" t="s">
+      <c r="AC25" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="AB25" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC25" s="46" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="26" spans="1:29" ht="21.95" customHeight="1">
+    <row r="26" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="36"/>
+        <v>53</v>
+      </c>
+      <c r="B26" s="60"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="61"/>
       <c r="F26" s="16"/>
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
@@ -2672,50 +2675,50 @@
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
       <c r="M26" s="18"/>
-      <c r="N26" s="46" t="s">
+      <c r="N26" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="O26" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="P26" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="O26" s="46" t="s">
+      <c r="Q26" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P26" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q26" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="R26" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="S26" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="T26" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="U26" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="V26" s="43"/>
-      <c r="W26" s="44"/>
-      <c r="X26" s="44"/>
-      <c r="Y26" s="45"/>
-      <c r="Z26" s="46" t="s">
+      <c r="R26" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="S26" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="T26" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="U26" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="V26" s="38"/>
+      <c r="W26" s="39"/>
+      <c r="X26" s="39"/>
+      <c r="Y26" s="40"/>
+      <c r="Z26" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA26" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB26" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="AA26" s="46" t="s">
+      <c r="AC26" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="AB26" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC26" s="46" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="27" spans="1:29" ht="21.95" customHeight="1">
+    <row r="27" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
@@ -2746,9 +2749,9 @@
       <c r="AB27" s="7"/>
       <c r="AC27" s="6"/>
     </row>
-    <row r="28" spans="1:29" ht="21.95" customHeight="1">
+    <row r="28" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
@@ -2779,9 +2782,9 @@
       <c r="AB28" s="7"/>
       <c r="AC28" s="6"/>
     </row>
-    <row r="29" spans="1:29" ht="21.95" customHeight="1">
+    <row r="29" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
@@ -2825,23 +2828,22 @@
     <mergeCell ref="Z8:AA11"/>
     <mergeCell ref="AB8:AC11"/>
     <mergeCell ref="B8:C15"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="V8:Y11"/>
+    <mergeCell ref="X12:Y15"/>
+    <mergeCell ref="Z12:AC15"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
-    <mergeCell ref="N19:O22"/>
-    <mergeCell ref="P19:Q22"/>
-    <mergeCell ref="F10:I11"/>
-    <mergeCell ref="F12:G15"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="P23:Q26"/>
-    <mergeCell ref="R23:S26"/>
-    <mergeCell ref="T23:U26"/>
+    <mergeCell ref="B19:C26"/>
+    <mergeCell ref="D19:E26"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="V12:W15"/>
     <mergeCell ref="R12:S15"/>
     <mergeCell ref="AA1:AC1"/>
@@ -2856,11 +2858,8 @@
     <mergeCell ref="N7:U7"/>
     <mergeCell ref="V6:AC6"/>
     <mergeCell ref="V7:AC7"/>
-    <mergeCell ref="B19:C26"/>
-    <mergeCell ref="D19:E26"/>
-    <mergeCell ref="V8:Y11"/>
-    <mergeCell ref="X12:Y15"/>
-    <mergeCell ref="Z12:AC15"/>
+    <mergeCell ref="F10:I11"/>
+    <mergeCell ref="F12:G15"/>
     <mergeCell ref="X19:Y22"/>
     <mergeCell ref="Z19:AC22"/>
     <mergeCell ref="V23:Y26"/>
@@ -2872,6 +2871,10 @@
     <mergeCell ref="R19:U22"/>
     <mergeCell ref="V19:W22"/>
     <mergeCell ref="N23:O26"/>
+    <mergeCell ref="R23:S26"/>
+    <mergeCell ref="T23:U26"/>
+    <mergeCell ref="N19:O22"/>
+    <mergeCell ref="P19:Q22"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>